<commit_message>
-Read File -Get Section from file -Convert file in Object -Parse Object in JSON (import GSON)
</commit_message>
<xml_diff>
--- a/src/main/resources/static/Esempio_del_file_excel_esportato_da_cassa_19_Luglio_2022.xlsx
+++ b/src/main/resources/static/Esempio_del_file_excel_esportato_da_cassa_19_Luglio_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matteoprovezza/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giusepperaddato/IdeaProjects/AcademyJavaXIV/XLSXmanager/src/main/resources/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{707223C9-A2B9-854B-92BF-F046EE62E66A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFB1682-BE2C-9C4D-AF1D-C2ACA8C8673C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19880"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio 1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="182">
   <si>
     <t>Zmenu - Daily report</t>
   </si>
@@ -574,13 +574,16 @@
     <t>10:37</t>
   </si>
   <si>
-    <t>prova</t>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -627,7 +630,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -640,8 +643,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -688,11 +709,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -708,6 +738,30 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -721,9 +775,28 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -744,16 +817,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1067,15 +1130,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F138"/>
+  <dimension ref="A1:F136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="201" zoomScaleNormal="201" workbookViewId="0">
-      <selection activeCell="D138" sqref="D138"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="132" zoomScaleNormal="201" workbookViewId="0">
+      <selection activeCell="A135" sqref="A135:XFD135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1101,74 +1164,74 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="7"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="9" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="20"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="9" t="s">
+      <c r="B7" s="20"/>
+      <c r="C7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="20"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="17"/>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -1181,114 +1244,114 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="11" t="s">
+      <c r="B14" s="17"/>
+      <c r="C14" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="11" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="17"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="11" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="7"/>
+      <c r="D16" s="17"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="11" t="s">
+      <c r="B17" s="17"/>
+      <c r="C17" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="17"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="11" t="s">
+      <c r="B19" s="17"/>
+      <c r="C19" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="D19" s="17"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="11" t="s">
+      <c r="B20" s="17"/>
+      <c r="C20" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="7"/>
+      <c r="D20" s="17"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="11" t="s">
+      <c r="B21" s="17"/>
+      <c r="C21" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="7"/>
+      <c r="D21" s="17"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="11" t="s">
+      <c r="B23" s="17"/>
+      <c r="C23" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="7"/>
+      <c r="D23" s="17"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="11" t="s">
+      <c r="B24" s="17"/>
+      <c r="C24" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="7"/>
+      <c r="D24" s="17"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="11" t="s">
+      <c r="B25" s="17"/>
+      <c r="C25" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="17"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="11" t="s">
+      <c r="B26" s="17"/>
+      <c r="C26" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="7"/>
+      <c r="D26" s="17"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
@@ -1296,12 +1359,12 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="7"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="17"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
@@ -1337,104 +1400,104 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="11" t="s">
+      <c r="B35" s="17"/>
+      <c r="C35" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="7"/>
+      <c r="D35" s="17"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="11" t="s">
+      <c r="B36" s="17"/>
+      <c r="C36" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="7"/>
+      <c r="D36" s="17"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="11" t="s">
+      <c r="B37" s="17"/>
+      <c r="C37" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="7"/>
+      <c r="D37" s="17"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="11" t="s">
+      <c r="B39" s="17"/>
+      <c r="C39" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="7"/>
+      <c r="D39" s="17"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="11" t="s">
+      <c r="B40" s="17"/>
+      <c r="C40" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D40" s="7"/>
+      <c r="D40" s="17"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="11" t="s">
+      <c r="B41" s="17"/>
+      <c r="C41" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="7"/>
+      <c r="D41" s="17"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="11" t="s">
+      <c r="B43" s="17"/>
+      <c r="C43" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="7"/>
+      <c r="D43" s="17"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="11" t="s">
+      <c r="B44" s="17"/>
+      <c r="C44" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="7"/>
+      <c r="D44" s="17"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="11" t="s">
+      <c r="B45" s="17"/>
+      <c r="C45" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="7"/>
+      <c r="D45" s="17"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="11" t="s">
+      <c r="B47" s="17"/>
+      <c r="C47" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D47" s="7"/>
+      <c r="D47" s="17"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
@@ -1442,54 +1505,54 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="11" t="s">
+      <c r="B50" s="17"/>
+      <c r="C50" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D50" s="7"/>
+      <c r="D50" s="17"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="11" t="s">
+      <c r="B51" s="17"/>
+      <c r="C51" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D51" s="7"/>
+      <c r="D51" s="17"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="11" t="s">
+      <c r="B52" s="17"/>
+      <c r="C52" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D52" s="7"/>
+      <c r="D52" s="17"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="7"/>
-      <c r="C53" s="11" t="s">
+      <c r="B53" s="17"/>
+      <c r="C53" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D53" s="7"/>
+      <c r="D53" s="17"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B54" s="7"/>
-      <c r="C54" s="11" t="s">
+      <c r="B54" s="17"/>
+      <c r="C54" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D54" s="7"/>
+      <c r="D54" s="17"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" s="2" t="s">
@@ -1497,34 +1560,34 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="7"/>
-      <c r="C57" s="11" t="s">
+      <c r="B57" s="17"/>
+      <c r="C57" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D57" s="7"/>
+      <c r="D57" s="17"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="7"/>
-      <c r="C58" s="11" t="s">
+      <c r="B58" s="17"/>
+      <c r="C58" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D58" s="7"/>
+      <c r="D58" s="17"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B59" s="7"/>
-      <c r="C59" s="11" t="s">
+      <c r="B59" s="17"/>
+      <c r="C59" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D59" s="7"/>
+      <c r="D59" s="17"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
@@ -1538,10 +1601,10 @@
       <c r="B62" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="12" t="s">
+      <c r="C62" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D62" s="7"/>
+      <c r="D62" s="17"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" s="4" t="s">
@@ -1550,10 +1613,10 @@
       <c r="B63" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="11" t="s">
+      <c r="C63" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="D63" s="7"/>
+      <c r="D63" s="17"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" s="4" t="s">
@@ -1562,211 +1625,239 @@
       <c r="B64" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C64" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D64" s="7"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="6" t="s">
+      <c r="D64" s="17"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A65" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B65" s="7"/>
-      <c r="C65" s="11" t="s">
+      <c r="B65" s="17"/>
+      <c r="C65" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="7"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D65" s="17"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A67" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="6" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A68" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B68" s="7"/>
-      <c r="C68" s="11" t="s">
+      <c r="B68" s="17"/>
+      <c r="C68" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D68" s="7"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="6" t="s">
+      <c r="D68" s="17"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A69" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B69" s="7"/>
-      <c r="C69" s="11" t="s">
+      <c r="B69" s="17"/>
+      <c r="C69" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D69" s="7"/>
-    </row>
-    <row r="71" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="D69" s="17"/>
+    </row>
+    <row r="71" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A72" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="2" t="s">
+    <row r="74" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A74" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A75" s="12" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A75" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B75" s="8"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="7"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A76" s="3" t="s">
+      <c r="B75" s="23"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="24"/>
+      <c r="E75" s="30" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A76" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C76" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="D76" s="7" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A77" s="5" t="s">
+      <c r="E76" s="30"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A77" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C77" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A79" s="12" t="s">
+      <c r="E77" s="30"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A78" s="6"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="30"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A79" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B79" s="8"/>
-      <c r="C79" s="8"/>
-      <c r="D79" s="7"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A80" s="3" t="s">
+      <c r="B79" s="23"/>
+      <c r="C79" s="23"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="30"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A80" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="C80" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D80" s="4" t="s">
+      <c r="D80" s="9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A81" s="4" t="s">
+      <c r="E80" s="30"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A81" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C81" s="5" t="s">
+      <c r="C81" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D81" s="8" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A82" s="12" t="s">
+      <c r="E81" s="30"/>
+    </row>
+    <row r="82" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A82" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="B82" s="8"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="7"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A83" s="3" t="s">
+      <c r="B82" s="26"/>
+      <c r="C82" s="26"/>
+      <c r="D82" s="27"/>
+      <c r="E82" s="30"/>
+    </row>
+    <row r="83" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A83" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C83" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="D83" s="11" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A84" s="5" t="s">
+      <c r="E83" s="30"/>
+    </row>
+    <row r="84" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A84" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C84" s="5" t="s">
+      <c r="C84" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D84" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A86" s="12" t="s">
+      <c r="E84" s="30"/>
+    </row>
+    <row r="85" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="13"/>
+      <c r="B85" s="13"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="30"/>
+    </row>
+    <row r="86" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A86" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B86" s="8"/>
-      <c r="C86" s="8"/>
-      <c r="D86" s="7"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A87" s="3" t="s">
+      <c r="B86" s="26"/>
+      <c r="C86" s="26"/>
+      <c r="D86" s="27"/>
+      <c r="E86" s="30"/>
+    </row>
+    <row r="87" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A87" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C87" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D87" s="4" t="s">
+      <c r="D87" s="14" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A88" s="4" t="s">
+      <c r="E87" s="30"/>
+    </row>
+    <row r="88" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A88" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C88" s="5" t="s">
+      <c r="C88" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D88" s="12" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E88" s="30"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A90" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A91" s="3" t="s">
         <v>59</v>
       </c>
@@ -1776,22 +1867,26 @@
       <c r="C91" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A92" s="6" t="s">
+      <c r="D91" s="31" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A92" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B92" s="7"/>
+      <c r="B92" s="17"/>
       <c r="C92" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D92" s="31"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A94" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A95" s="3" t="s">
         <v>59</v>
       </c>
@@ -1802,7 +1897,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A96" s="4" t="s">
         <v>88</v>
       </c>
@@ -1825,10 +1920,10 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A98" s="6" t="s">
+      <c r="A98" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B98" s="7"/>
+      <c r="B98" s="17"/>
       <c r="C98" s="5" t="s">
         <v>22</v>
       </c>
@@ -1917,12 +2012,12 @@
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A109" s="6" t="s">
+      <c r="A109" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B109" s="8"/>
-      <c r="C109" s="8"/>
-      <c r="D109" s="7"/>
+      <c r="B109" s="18"/>
+      <c r="C109" s="18"/>
+      <c r="D109" s="17"/>
       <c r="E109" s="5" t="s">
         <v>30</v>
       </c>
@@ -1933,375 +2028,355 @@
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A112" s="13" t="s">
+      <c r="A112" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="B112" s="13" t="s">
+      <c r="B112" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C112" s="13" t="s">
+      <c r="C112" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="D112" s="13" t="s">
+      <c r="D112" s="32" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A113" s="14" t="s">
+      <c r="A113" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="B113" s="14" t="s">
+      <c r="B113" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="C113" s="15" t="s">
+      <c r="C113" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="D113" s="15" t="s">
+      <c r="D113" s="34" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A114" s="16" t="s">
+      <c r="A114" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="B114" s="16" t="s">
+      <c r="B114" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="C114" s="17" t="s">
+      <c r="C114" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="D114" s="17" t="s">
+      <c r="D114" s="36" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A115" s="16" t="s">
+      <c r="A115" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="B115" s="16" t="s">
+      <c r="B115" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="C115" s="17" t="s">
+      <c r="C115" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D115" s="17" t="s">
+      <c r="D115" s="36" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A116" s="16" t="s">
+      <c r="A116" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="B116" s="16" t="s">
+      <c r="B116" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="C116" s="17" t="s">
+      <c r="C116" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D116" s="17" t="s">
+      <c r="D116" s="36" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A117" s="16" t="s">
+      <c r="A117" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="B117" s="16" t="s">
+      <c r="B117" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="C117" s="17" t="s">
+      <c r="C117" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D117" s="17" t="s">
+      <c r="D117" s="36" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A118" s="16" t="s">
+      <c r="A118" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="B118" s="16" t="s">
+      <c r="B118" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="C118" s="17" t="s">
+      <c r="C118" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="D118" s="17" t="s">
+      <c r="D118" s="36" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A119" s="16" t="s">
+      <c r="A119" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="B119" s="16" t="s">
+      <c r="B119" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="C119" s="17" t="s">
+      <c r="C119" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="D119" s="17" t="s">
+      <c r="D119" s="36" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A120" s="16" t="s">
+      <c r="A120" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="B120" s="16" t="s">
+      <c r="B120" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="C120" s="17" t="s">
+      <c r="C120" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D120" s="17" t="s">
+      <c r="D120" s="36" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A121" s="16" t="s">
+      <c r="A121" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="B121" s="16" t="s">
+      <c r="B121" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="C121" s="17" t="s">
+      <c r="C121" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="D121" s="17" t="s">
+      <c r="D121" s="36" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A122" s="16" t="s">
+      <c r="A122" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="B122" s="16" t="s">
+      <c r="B122" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="C122" s="17" t="s">
+      <c r="C122" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D122" s="17" t="s">
+      <c r="D122" s="36" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A123" s="14" t="s">
+      <c r="A123" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="B123" s="14" t="s">
+      <c r="B123" s="33" t="s">
         <v>145</v>
       </c>
-      <c r="C123" s="15" t="s">
+      <c r="C123" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="D123" s="15" t="s">
+      <c r="D123" s="34" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A124" s="16" t="s">
+      <c r="A124" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="B124" s="16" t="s">
+      <c r="B124" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="C124" s="17" t="s">
+      <c r="C124" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D124" s="17" t="s">
+      <c r="D124" s="36" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A125" s="16" t="s">
+      <c r="A125" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="B125" s="16" t="s">
+      <c r="B125" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="C125" s="17" t="s">
+      <c r="C125" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="D125" s="17" t="s">
+      <c r="D125" s="36" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A126" s="16" t="s">
+      <c r="A126" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="B126" s="16" t="s">
+      <c r="B126" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="C126" s="17" t="s">
+      <c r="C126" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D126" s="17" t="s">
+      <c r="D126" s="36" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A127" s="16" t="s">
+      <c r="A127" s="35" t="s">
         <v>155</v>
       </c>
-      <c r="B127" s="16" t="s">
+      <c r="B127" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="C127" s="17" t="s">
+      <c r="C127" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="D127" s="17" t="s">
+      <c r="D127" s="36" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A128" s="16" t="s">
+      <c r="A128" s="35" t="s">
         <v>159</v>
       </c>
-      <c r="B128" s="16" t="s">
+      <c r="B128" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="C128" s="17" t="s">
+      <c r="C128" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D128" s="17" t="s">
+      <c r="D128" s="36" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A129" s="14" t="s">
+      <c r="A129" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="B129" s="14" t="s">
+      <c r="B129" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="C129" s="15" t="s">
+      <c r="C129" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="D129" s="15" t="s">
+      <c r="D129" s="34" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A130" s="16" t="s">
+      <c r="A130" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="B130" s="16" t="s">
+      <c r="B130" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="C130" s="17" t="s">
+      <c r="C130" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D130" s="17" t="s">
+      <c r="D130" s="36" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A131" s="16" t="s">
+      <c r="A131" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="B131" s="16" t="s">
+      <c r="B131" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="C131" s="17" t="s">
+      <c r="C131" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D131" s="17" t="s">
+      <c r="D131" s="36" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A132" s="16" t="s">
+      <c r="A132" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="B132" s="16" t="s">
+      <c r="B132" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="C132" s="17" t="s">
+      <c r="C132" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="D132" s="17" t="s">
+      <c r="D132" s="36" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A133" s="16" t="s">
+      <c r="A133" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="B133" s="16" t="s">
+      <c r="B133" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="C133" s="17" t="s">
+      <c r="C133" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="D133" s="17" t="s">
+      <c r="D133" s="36" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A134" s="14" t="s">
+      <c r="A134" s="33" t="s">
         <v>174</v>
       </c>
-      <c r="B134" s="14" t="s">
+      <c r="B134" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="C134" s="15" t="s">
+      <c r="C134" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="D134" s="15" t="s">
+      <c r="D134" s="34" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A135" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="B135" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="C135" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="D135" s="22" t="s">
-        <v>180</v>
+      <c r="A135" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="B135" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="C135" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="D135" s="36" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A136" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="B136" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="C136" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="D136" s="17" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A137" s="18" t="s">
+      <c r="A136" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B137" s="19"/>
-      <c r="C137" s="20"/>
-      <c r="D137" s="17" t="s">
+      <c r="B136" s="38"/>
+      <c r="C136" s="39"/>
+      <c r="D136" s="36" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A138" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="D138" s="24">
-        <v>1234</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="90">
+  <mergeCells count="92">
+    <mergeCell ref="E75:E88"/>
+    <mergeCell ref="D91:D92"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="A4:B4"/>
@@ -2385,7 +2460,7 @@
     <mergeCell ref="A92:B92"/>
     <mergeCell ref="A98:B98"/>
     <mergeCell ref="A109:D109"/>
-    <mergeCell ref="A137:C137"/>
+    <mergeCell ref="A136:C136"/>
     <mergeCell ref="A69:B69"/>
     <mergeCell ref="C69:D69"/>
     <mergeCell ref="A75:D75"/>

</xml_diff>

<commit_message>
adding Transazioni, TransazioniSospese, TipoDiServizio, Sconto, Pagamento and update XLSXManager
</commit_message>
<xml_diff>
--- a/src/main/resources/static/Esempio_del_file_excel_esportato_da_cassa_19_Luglio_2022.xlsx
+++ b/src/main/resources/static/Esempio_del_file_excel_esportato_da_cassa_19_Luglio_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giusepperaddato/IdeaProjects/AcademyJavaXIV/XLSXmanager/src/main/resources/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless_in4zoow\IdeaProjects\XLSXmanager\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFB1682-BE2C-9C4D-AF1D-C2ACA8C8673C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA77B12-33E6-4471-A6B6-AB27D226F954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio 1" sheetId="1" r:id="rId1"/>
@@ -630,7 +630,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -658,6 +658,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -722,7 +728,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -763,18 +769,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -785,38 +824,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1137,22 +1144,22 @@
   </sheetPr>
   <dimension ref="A1:F136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="132" zoomScaleNormal="201" workbookViewId="0">
-      <selection activeCell="A135" sqref="A135:XFD135"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="132" zoomScaleNormal="201" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95:D98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="35.1640625" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="35.109375" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
-    <col min="6" max="6" width="9.5" customWidth="1"/>
-    <col min="7" max="256" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="7" max="256" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1163,210 +1170,217 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="21" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="17"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="16" t="s">
+      <c r="D3" s="25"/>
+      <c r="E3" s="21"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="21" t="s">
+      <c r="B4" s="25"/>
+      <c r="C4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="17"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="16" t="s">
+      <c r="D4" s="25"/>
+      <c r="E4" s="21"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="21" t="s">
+      <c r="B5" s="25"/>
+      <c r="C5" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="17"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="19" t="s">
+      <c r="D5" s="25"/>
+      <c r="E5" s="21"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="19" t="s">
+      <c r="B6" s="28"/>
+      <c r="C6" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="20"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="19" t="s">
+      <c r="D6" s="28"/>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="19" t="s">
+      <c r="B7" s="28"/>
+      <c r="C7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="20"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="19" t="s">
+      <c r="D7" s="28"/>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="19" t="s">
+      <c r="B8" s="28"/>
+      <c r="C8" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="20"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="16" t="s">
+      <c r="D8" s="28"/>
+      <c r="E8" s="21"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="16" t="s">
+      <c r="B9" s="25"/>
+      <c r="C9" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="17"/>
-    </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="D9" s="25"/>
+      <c r="E9" s="21"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="16" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="21" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="17"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="16" t="s">
+      <c r="D14" s="25"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="21" t="s">
+      <c r="B15" s="25"/>
+      <c r="C15" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="17"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" s="16" t="s">
+      <c r="D15" s="25"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="21" t="s">
+      <c r="B16" s="25"/>
+      <c r="C16" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="17"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="16" t="s">
+      <c r="D16" s="25"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="17"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="17"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="16" t="s">
+      <c r="D17" s="25"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="21" t="s">
+      <c r="B19" s="25"/>
+      <c r="C19" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="17"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="16" t="s">
+      <c r="D19" s="25"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="21" t="s">
+      <c r="B20" s="25"/>
+      <c r="C20" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="17"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="16" t="s">
+      <c r="D20" s="25"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="21" t="s">
+      <c r="B21" s="25"/>
+      <c r="C21" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="17"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="16" t="s">
+      <c r="D21" s="25"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="21" t="s">
+      <c r="B23" s="25"/>
+      <c r="C23" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="17"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A24" s="16" t="s">
+      <c r="D23" s="25"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="21" t="s">
+      <c r="B24" s="25"/>
+      <c r="C24" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="17"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="16" t="s">
+      <c r="D24" s="25"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="21" t="s">
+      <c r="B25" s="25"/>
+      <c r="C25" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="17"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="16" t="s">
+      <c r="D25" s="25"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="21" t="s">
+      <c r="B26" s="25"/>
+      <c r="C26" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="17"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D26" s="25"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="28" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="17"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="25"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>33</v>
       </c>
@@ -1380,7 +1394,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>36</v>
       </c>
@@ -1394,304 +1408,308 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="16" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="21" t="s">
+      <c r="B35" s="25"/>
+      <c r="C35" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D35" s="17"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="16" t="s">
+      <c r="D35" s="25"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="21" t="s">
+      <c r="B36" s="25"/>
+      <c r="C36" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="17"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="16" t="s">
+      <c r="D36" s="25"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="17"/>
-      <c r="C37" s="21" t="s">
+      <c r="B37" s="25"/>
+      <c r="C37" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="17"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A39" s="16" t="s">
+      <c r="D37" s="25"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="17"/>
-      <c r="C39" s="21" t="s">
+      <c r="B39" s="25"/>
+      <c r="C39" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="17"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A40" s="16" t="s">
+      <c r="D39" s="25"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="21" t="s">
+      <c r="B40" s="25"/>
+      <c r="C40" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D40" s="17"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="16" t="s">
+      <c r="D40" s="25"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="21" t="s">
+      <c r="B41" s="25"/>
+      <c r="C41" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="17"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A43" s="16" t="s">
+      <c r="D41" s="25"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="17"/>
-      <c r="C43" s="21" t="s">
+      <c r="B43" s="25"/>
+      <c r="C43" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D43" s="17"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A44" s="16" t="s">
+      <c r="D43" s="25"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="17"/>
-      <c r="C44" s="21" t="s">
+      <c r="B44" s="25"/>
+      <c r="C44" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="17"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="16" t="s">
+      <c r="D44" s="25"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="17"/>
-      <c r="C45" s="21" t="s">
+      <c r="B45" s="25"/>
+      <c r="C45" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="17"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="16" t="s">
+      <c r="D45" s="25"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="17"/>
-      <c r="C47" s="21" t="s">
+      <c r="B47" s="25"/>
+      <c r="C47" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D47" s="17"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D47" s="25"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="16" t="s">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="17"/>
-      <c r="C50" s="21" t="s">
+      <c r="B50" s="25"/>
+      <c r="C50" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D50" s="17"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A51" s="16" t="s">
+      <c r="D50" s="25"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="17"/>
-      <c r="C51" s="21" t="s">
+      <c r="B51" s="25"/>
+      <c r="C51" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D51" s="17"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A52" s="16" t="s">
+      <c r="D51" s="25"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="17"/>
-      <c r="C52" s="21" t="s">
+      <c r="B52" s="25"/>
+      <c r="C52" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D52" s="17"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A53" s="16" t="s">
+      <c r="D52" s="25"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="17"/>
-      <c r="C53" s="21" t="s">
+      <c r="B53" s="25"/>
+      <c r="C53" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D53" s="17"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A54" s="16" t="s">
+      <c r="D53" s="25"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B54" s="17"/>
-      <c r="C54" s="21" t="s">
+      <c r="B54" s="25"/>
+      <c r="C54" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D54" s="17"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D54" s="25"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A57" s="16" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="17"/>
-      <c r="C57" s="21" t="s">
+      <c r="B57" s="25"/>
+      <c r="C57" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D57" s="17"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="16" t="s">
+      <c r="D57" s="25"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="17"/>
-      <c r="C58" s="21" t="s">
+      <c r="B58" s="25"/>
+      <c r="C58" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D58" s="17"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="16" t="s">
+      <c r="D58" s="25"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B59" s="17"/>
-      <c r="C59" s="21" t="s">
+      <c r="B59" s="25"/>
+      <c r="C59" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D59" s="17"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D59" s="25"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="28" t="s">
+      <c r="C62" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D62" s="17"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D62" s="25"/>
+      <c r="E62" s="21"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="21" t="s">
+      <c r="C63" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="D63" s="17"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D63" s="25"/>
+      <c r="E63" s="21"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C64" s="21" t="s">
+      <c r="C64" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="D64" s="17"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A65" s="16" t="s">
+      <c r="D64" s="25"/>
+      <c r="E64" s="21"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B65" s="17"/>
-      <c r="C65" s="21" t="s">
+      <c r="B65" s="25"/>
+      <c r="C65" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="17"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D65" s="25"/>
+      <c r="E65" s="21"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A68" s="16" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B68" s="17"/>
-      <c r="C68" s="21" t="s">
+      <c r="B68" s="25"/>
+      <c r="C68" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D68" s="17"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A69" s="16" t="s">
+      <c r="D68" s="25"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B69" s="17"/>
-      <c r="C69" s="21" t="s">
+      <c r="B69" s="25"/>
+      <c r="C69" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D69" s="17"/>
-    </row>
-    <row r="71" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="D69" s="25"/>
+    </row>
+    <row r="71" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A75" s="22" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="B75" s="23"/>
-      <c r="C75" s="23"/>
-      <c r="D75" s="24"/>
-      <c r="E75" s="30" t="s">
+      <c r="B75" s="36"/>
+      <c r="C75" s="36"/>
+      <c r="D75" s="37"/>
+      <c r="E75" s="22" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>73</v>
       </c>
@@ -1704,9 +1722,9 @@
       <c r="D76" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E76" s="30"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E76" s="22"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
         <v>77</v>
       </c>
@@ -1719,25 +1737,25 @@
       <c r="D77" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="E77" s="30"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E77" s="22"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
-      <c r="E78" s="30"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A79" s="22" t="s">
+      <c r="E78" s="22"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B79" s="23"/>
-      <c r="C79" s="23"/>
-      <c r="D79" s="24"/>
-      <c r="E79" s="30"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B79" s="36"/>
+      <c r="C79" s="36"/>
+      <c r="D79" s="37"/>
+      <c r="E79" s="22"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>33</v>
       </c>
@@ -1750,9 +1768,9 @@
       <c r="D80" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E80" s="30"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E80" s="22"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>36</v>
       </c>
@@ -1765,18 +1783,18 @@
       <c r="D81" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E81" s="30"/>
-    </row>
-    <row r="82" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="25" t="s">
+      <c r="E81" s="22"/>
+    </row>
+    <row r="82" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="B82" s="26"/>
-      <c r="C82" s="26"/>
-      <c r="D82" s="27"/>
-      <c r="E82" s="30"/>
-    </row>
-    <row r="83" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B82" s="39"/>
+      <c r="C82" s="39"/>
+      <c r="D82" s="40"/>
+      <c r="E82" s="22"/>
+    </row>
+    <row r="83" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>73</v>
       </c>
@@ -1789,9 +1807,9 @@
       <c r="D83" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E83" s="30"/>
-    </row>
-    <row r="84" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="E83" s="22"/>
+    </row>
+    <row r="84" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
         <v>82</v>
       </c>
@@ -1804,25 +1822,25 @@
       <c r="D84" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E84" s="30"/>
-    </row>
-    <row r="85" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="E84" s="22"/>
+    </row>
+    <row r="85" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="13"/>
       <c r="B85" s="13"/>
       <c r="C85" s="13"/>
       <c r="D85" s="13"/>
-      <c r="E85" s="30"/>
-    </row>
-    <row r="86" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="25" t="s">
+      <c r="E85" s="22"/>
+    </row>
+    <row r="86" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="B86" s="26"/>
-      <c r="C86" s="26"/>
-      <c r="D86" s="27"/>
-      <c r="E86" s="30"/>
-    </row>
-    <row r="87" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B86" s="39"/>
+      <c r="C86" s="39"/>
+      <c r="D86" s="40"/>
+      <c r="E86" s="22"/>
+    </row>
+    <row r="87" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
         <v>33</v>
       </c>
@@ -1835,9 +1853,9 @@
       <c r="D87" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E87" s="30"/>
-    </row>
-    <row r="88" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="E87" s="22"/>
+    </row>
+    <row r="88" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
         <v>36</v>
       </c>
@@ -1850,14 +1868,14 @@
       <c r="D88" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="E88" s="30"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="E88" s="22"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>59</v>
       </c>
@@ -1867,26 +1885,26 @@
       <c r="C91" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D91" s="31" t="s">
+      <c r="D91" s="23" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A92" s="16" t="s">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B92" s="17"/>
+      <c r="B92" s="25"/>
       <c r="C92" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D92" s="31"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D92" s="23"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>59</v>
       </c>
@@ -1896,8 +1914,9 @@
       <c r="C95" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D95" s="21"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>88</v>
       </c>
@@ -1907,8 +1926,9 @@
       <c r="C96" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D96" s="21"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>90</v>
       </c>
@@ -1918,32 +1938,34 @@
       <c r="C97" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A98" s="16" t="s">
+      <c r="D97" s="21"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B98" s="17"/>
+      <c r="B98" s="25"/>
       <c r="C98" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D98" s="21"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>93</v>
       </c>
@@ -1959,8 +1981,9 @@
       <c r="E105" s="3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F105" s="21"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>98</v>
       </c>
@@ -1976,8 +1999,9 @@
       <c r="E106" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F106" s="21"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>98</v>
       </c>
@@ -1993,8 +2017,9 @@
       <c r="E107" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F107" s="21"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>104</v>
       </c>
@@ -2010,371 +2035,474 @@
       <c r="E108" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A109" s="16" t="s">
+      <c r="F108" s="21"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B109" s="18"/>
-      <c r="C109" s="18"/>
-      <c r="D109" s="17"/>
+      <c r="B109" s="31"/>
+      <c r="C109" s="31"/>
+      <c r="D109" s="25"/>
       <c r="E109" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="F109" s="21"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A112" s="32" t="s">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="B112" s="32" t="s">
+      <c r="B112" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C112" s="32" t="s">
+      <c r="C112" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D112" s="32" t="s">
+      <c r="D112" s="16" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A113" s="33" t="s">
+      <c r="E112" s="21"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="B113" s="33" t="s">
+      <c r="B113" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="C113" s="34" t="s">
+      <c r="C113" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D113" s="34" t="s">
+      <c r="D113" s="18" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A114" s="35" t="s">
+      <c r="E113" s="21"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="B114" s="35" t="s">
+      <c r="B114" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="C114" s="36" t="s">
+      <c r="C114" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="D114" s="36" t="s">
+      <c r="D114" s="20" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A115" s="35" t="s">
+      <c r="E114" s="21"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="B115" s="35" t="s">
+      <c r="B115" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C115" s="36" t="s">
+      <c r="C115" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D115" s="36" t="s">
+      <c r="D115" s="20" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A116" s="35" t="s">
+      <c r="E115" s="21"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="B116" s="35" t="s">
+      <c r="B116" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="C116" s="36" t="s">
+      <c r="C116" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D116" s="36" t="s">
+      <c r="D116" s="20" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A117" s="35" t="s">
+      <c r="E116" s="21"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="B117" s="35" t="s">
+      <c r="B117" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="C117" s="36" t="s">
+      <c r="C117" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D117" s="36" t="s">
+      <c r="D117" s="20" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A118" s="35" t="s">
+      <c r="E117" s="21"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="B118" s="35" t="s">
+      <c r="B118" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="C118" s="36" t="s">
+      <c r="C118" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="D118" s="36" t="s">
+      <c r="D118" s="20" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A119" s="35" t="s">
+      <c r="E118" s="21"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="B119" s="35" t="s">
+      <c r="B119" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C119" s="36" t="s">
+      <c r="C119" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="D119" s="36" t="s">
+      <c r="D119" s="20" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A120" s="35" t="s">
+      <c r="E119" s="21"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="B120" s="35" t="s">
+      <c r="B120" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="C120" s="36" t="s">
+      <c r="C120" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D120" s="36" t="s">
+      <c r="D120" s="20" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A121" s="35" t="s">
+      <c r="E120" s="21"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B121" s="35" t="s">
+      <c r="B121" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="C121" s="36" t="s">
+      <c r="C121" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="D121" s="36" t="s">
+      <c r="D121" s="20" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A122" s="35" t="s">
+      <c r="E121" s="21"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="B122" s="35" t="s">
+      <c r="B122" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="C122" s="36" t="s">
+      <c r="C122" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D122" s="36" t="s">
+      <c r="D122" s="20" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A123" s="33" t="s">
+      <c r="E122" s="21"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="B123" s="33" t="s">
+      <c r="B123" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="C123" s="34" t="s">
+      <c r="C123" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="D123" s="34" t="s">
+      <c r="D123" s="18" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A124" s="35" t="s">
+      <c r="E123" s="21"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="B124" s="35" t="s">
+      <c r="B124" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="C124" s="36" t="s">
+      <c r="C124" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D124" s="36" t="s">
+      <c r="D124" s="20" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A125" s="35" t="s">
+      <c r="E124" s="21"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="B125" s="35" t="s">
+      <c r="B125" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="C125" s="36" t="s">
+      <c r="C125" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="D125" s="36" t="s">
+      <c r="D125" s="20" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A126" s="35" t="s">
+      <c r="E125" s="21"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="B126" s="35" t="s">
+      <c r="B126" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="C126" s="36" t="s">
+      <c r="C126" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D126" s="36" t="s">
+      <c r="D126" s="20" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A127" s="35" t="s">
+      <c r="E126" s="21"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="B127" s="35" t="s">
+      <c r="B127" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="C127" s="36" t="s">
+      <c r="C127" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="D127" s="36" t="s">
+      <c r="D127" s="20" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A128" s="35" t="s">
+      <c r="E127" s="21"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="B128" s="35" t="s">
+      <c r="B128" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="C128" s="36" t="s">
+      <c r="C128" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D128" s="36" t="s">
+      <c r="D128" s="20" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A129" s="33" t="s">
+      <c r="E128" s="21"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="B129" s="33" t="s">
+      <c r="B129" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="C129" s="34" t="s">
+      <c r="C129" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="D129" s="34" t="s">
+      <c r="D129" s="18" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A130" s="35" t="s">
+      <c r="E129" s="21"/>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="B130" s="35" t="s">
+      <c r="B130" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="C130" s="36" t="s">
+      <c r="C130" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D130" s="36" t="s">
+      <c r="D130" s="20" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A131" s="35" t="s">
+      <c r="E130" s="21"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="B131" s="35" t="s">
+      <c r="B131" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="C131" s="36" t="s">
+      <c r="C131" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D131" s="36" t="s">
+      <c r="D131" s="20" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A132" s="35" t="s">
+      <c r="E131" s="21"/>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="B132" s="35" t="s">
+      <c r="B132" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="C132" s="36" t="s">
+      <c r="C132" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D132" s="36" t="s">
+      <c r="D132" s="20" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A133" s="35" t="s">
+      <c r="E132" s="21"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="B133" s="35" t="s">
+      <c r="B133" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="C133" s="36" t="s">
+      <c r="C133" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="D133" s="36" t="s">
+      <c r="D133" s="20" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A134" s="33" t="s">
+      <c r="E133" s="21"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="B134" s="33" t="s">
+      <c r="B134" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="C134" s="34" t="s">
+      <c r="C134" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D134" s="34" t="s">
+      <c r="D134" s="18" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A135" s="35" t="s">
+      <c r="E134" s="21"/>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="B135" s="35" t="s">
+      <c r="B135" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="C135" s="36" t="s">
+      <c r="C135" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="D135" s="36" t="s">
+      <c r="D135" s="20" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A136" s="37" t="s">
+      <c r="E135" s="21"/>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B136" s="38"/>
-      <c r="C136" s="39"/>
-      <c r="D136" s="36" t="s">
+      <c r="B136" s="33"/>
+      <c r="C136" s="34"/>
+      <c r="D136" s="20" t="s">
         <v>22</v>
       </c>
+      <c r="E136" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="92">
+    <mergeCell ref="A136:C136"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="A86:D86"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A109:D109"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:D16"/>
     <mergeCell ref="E75:E88"/>
     <mergeCell ref="D91:D92"/>
     <mergeCell ref="A3:B3"/>
@@ -2391,82 +2519,6 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A109:D109"/>
-    <mergeCell ref="A136:C136"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A82:D82"/>
-    <mergeCell ref="A86:D86"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>